<commit_message>
Work plan ver.2 and design document
</commit_message>
<xml_diff>
--- a/Trading visualization assignment - Work plan.xlsx
+++ b/Trading visualization assignment - Work plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Create additional control objects  for showing technical indicators</t>
   </si>
@@ -77,13 +77,122 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>Downloaded and installed SciChart trial, together with the documentation</t>
+  </si>
+  <si>
+    <t>DAY 0</t>
+  </si>
+  <si>
+    <t>DAY 1</t>
+  </si>
+  <si>
+    <t>Created GitHub account and my first repository</t>
+  </si>
+  <si>
+    <t>Reviewed SciChart examples and introduced myself with tool's basic documentation and possibilities</t>
+  </si>
+  <si>
+    <t>Recognized following examples as potentially useful for my assignment:</t>
+  </si>
+  <si>
+    <t>Basic charts (line and candlestick)</t>
+  </si>
+  <si>
+    <t>Stock charts (realtime ticking stock chart)</t>
+  </si>
+  <si>
+    <t>Modify axis behavior (Modify axis properties)</t>
+  </si>
+  <si>
+    <t>Manipulate series (Change render series type)</t>
+  </si>
+  <si>
+    <t>Determined that WPF window can hold all of the required controls</t>
+  </si>
+  <si>
+    <t>Downloaded freely available data samples from different web sites. All of these sites ofer stock price and volume changes on daily basis (OHLC).</t>
+  </si>
+  <si>
+    <t>Downloaded stock data sample (whole year 2012 - subject to a change) for: Microsoft, Google, Cisco, Citybank, Coca Cola, McDonald's, Walt Disney co.</t>
+  </si>
+  <si>
+    <t>Started with a basic line chart as a template for my assignment and embeded it into my solution</t>
+  </si>
+  <si>
+    <t>Cerated a function 'private void ReadStockData(String sFileName)' to read a data source file and to set that data as a basis for the chart</t>
+  </si>
+  <si>
+    <t>Referenced SciChart library within the project</t>
+  </si>
+  <si>
+    <t>Created a new WPF C# project named "TradingVisualizationAssignment"</t>
+  </si>
+  <si>
+    <t>DAY 2</t>
+  </si>
+  <si>
+    <t>DAY 1 &amp; DAY 2</t>
+  </si>
+  <si>
+    <t>Because of the problem with DateTime data type, switched from a basic line chart as a template to FastCandlestickRenderableSeries and extended it with some additional parameters</t>
+  </si>
+  <si>
+    <t>Introduced DateTime type data as the X axis base - for a single stock, with no possibility to choose</t>
+  </si>
+  <si>
+    <t>Canceled the idea to introduce the scaling of the chart in order to corespond to data values - it is performed automatically</t>
+  </si>
+  <si>
+    <t>The step of showing several prices at the same time (open, high, low and close price) is skipped - performed automatically by the SciChart</t>
+  </si>
+  <si>
+    <t>Created a combo-box control that allows user to choose between the stocks</t>
+  </si>
+  <si>
+    <t>Passing the name of the file (combo-box argument) as a parameter to the previously created function changes data source and refreshes the SciChart position</t>
+  </si>
+  <si>
+    <t>In order to preserve what's been done previously, started a new C# WPF project - "Test"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Found the possible reason for the problems with the previous project - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ISSUE: data source must be presorted in order for SciChart to work correctly</t>
+    </r>
+  </si>
+  <si>
+    <t>Initial problems with documentation</t>
+  </si>
+  <si>
+    <t>Cannot switch X axis from double to DateTime</t>
+  </si>
+  <si>
+    <t>Started working with a different type of SciChart</t>
+  </si>
+  <si>
+    <t>Found the reason and overcame the problem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +201,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -259,19 +389,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -497,19 +614,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -540,7 +644,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -556,6 +660,70 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -569,16 +737,63 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -589,14 +804,126 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,128 +931,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,16 +1274,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <pane ySplit="24" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -1101,306 +1350,443 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10" t="s">
+    <row r="9" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="15"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="54"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="67"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="23"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="70"/>
+    </row>
+    <row r="13" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+      <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="31"/>
-    </row>
-    <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="32" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="64"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="31"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="63"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="36" t="s">
+      <c r="B15" s="50"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="31"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="24"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38" t="s">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="64"/>
+    </row>
+    <row r="16" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="31"/>
-    </row>
-    <row r="17" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="40" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="63"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="31"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="64"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="41" t="s">
+      <c r="B18" s="50"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="31"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="24"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="42" t="s">
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="63"/>
+    </row>
+    <row r="19" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="31"/>
-    </row>
-    <row r="20" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="43" t="s">
+      <c r="I19" s="21"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="64"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="34"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="31"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="46" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="31"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="24"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="48" t="s">
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
+    </row>
+    <row r="22" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="51"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="31"/>
-    </row>
-    <row r="23" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="52"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="55"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="45"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C24" s="40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="39"/>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="41"/>
+      <c r="C28" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="41"/>
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="41"/>
+      <c r="D30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="41"/>
+      <c r="D31" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="41"/>
+      <c r="D32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="41"/>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="41"/>
+      <c r="C34" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="41"/>
+      <c r="C35" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="41"/>
+      <c r="C36" s="56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="41"/>
+      <c r="C37" s="56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="41"/>
+      <c r="C38" s="56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="41"/>
+      <c r="C41" s="56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="41"/>
+      <c r="C42" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="41"/>
+      <c r="C43" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="41"/>
+      <c r="C44" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="58"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="41"/>
+      <c r="C45" s="57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="41"/>
+      <c r="C46" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="39"/>
+      <c r="C47" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
+  <mergeCells count="18">
+    <mergeCell ref="J14:O15"/>
+    <mergeCell ref="J16:O17"/>
+    <mergeCell ref="J11:O13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
     <mergeCell ref="N21:O21"/>
     <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="J18:O19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Newer versions of files
</commit_message>
<xml_diff>
--- a/Trading visualization assignment - Work plan.xlsx
+++ b/Trading visualization assignment - Work plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Create additional control objects  for showing technical indicators</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>Found the reason and overcame the problem</t>
+  </si>
+  <si>
+    <t>DAY 3</t>
+  </si>
+  <si>
+    <t>In order to use "Select folder dialog" referenced System.Windows.Forms</t>
+  </si>
+  <si>
+    <t>Introduced "Select folder dialog" so the user has to choose the starting folder, where all of the data is located</t>
+  </si>
+  <si>
+    <t>Applied the approach to show the names of data files without file extensions</t>
+  </si>
+  <si>
+    <t>Changed ReadStockData - much more elegant code...now it splits file into an array of string rows and each of them into arrays of string elements</t>
   </si>
 </sst>
 </file>
@@ -892,48 +907,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -943,15 +916,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -972,6 +945,48 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1274,11 +1289,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="24" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1374,17 +1389,17 @@
       <c r="I10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="52" t="s">
+      <c r="J10" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="61"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="62" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1396,17 +1411,17 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="65" t="s">
+      <c r="J11" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="67"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="50"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
@@ -1416,15 +1431,15 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="70"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="56"/>
     </row>
     <row r="13" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="50"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -1434,15 +1449,15 @@
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="64"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="50"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="57" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
@@ -1454,17 +1469,17 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="63"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="47"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="50"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25" t="s">
         <v>13</v>
@@ -1474,15 +1489,15 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="64"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="50"/>
     </row>
     <row r="16" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="50"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="26"/>
       <c r="D16" s="20"/>
       <c r="E16" s="27" t="s">
@@ -1492,17 +1507,17 @@
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="59" t="s">
+      <c r="J16" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="63"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="47"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="22"/>
@@ -1514,15 +1529,15 @@
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="64"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="50"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="50"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="24"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1532,17 +1547,17 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="59" t="s">
+      <c r="J18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="63"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="47"/>
     </row>
     <row r="19" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="50"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="26"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1552,15 +1567,15 @@
         <v>13</v>
       </c>
       <c r="I19" s="21"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="64"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="50"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="57" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="31"/>
@@ -1572,15 +1587,15 @@
       <c r="I20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="46"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="43"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="69"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="50"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="34"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1590,15 +1605,15 @@
       <c r="I21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="46"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="69"/>
     </row>
     <row r="22" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="36"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -1608,12 +1623,12 @@
       <c r="I22" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="45"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="70"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C24" s="40" t="s">
@@ -1692,19 +1707,19 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="41"/>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="42" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="41"/>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="42" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="41"/>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="42" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1726,13 +1741,13 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="41"/>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="41"/>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="42" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1744,14 +1759,14 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="41"/>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="H44" s="58"/>
+      <c r="H44" s="44"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="41"/>
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="43" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1767,26 +1782,52 @@
         <v>46</v>
       </c>
     </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="41"/>
+      <c r="C49" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="41"/>
+      <c r="C50" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="39"/>
+      <c r="C51" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="J18:O19"/>
     <mergeCell ref="J14:O15"/>
     <mergeCell ref="J16:O17"/>
     <mergeCell ref="J11:O13"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
     <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N21:O21"/>
     <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="J18:O19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
New version of files
Additional controls embedded
New data structures used
There is no more requirement to presort data source files
</commit_message>
<xml_diff>
--- a/Trading visualization assignment - Work plan.xlsx
+++ b/Trading visualization assignment - Work plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Create additional control objects  for showing technical indicators</t>
   </si>
@@ -115,18 +115,9 @@
     <t>Determined that WPF window can hold all of the required controls</t>
   </si>
   <si>
-    <t>Downloaded freely available data samples from different web sites. All of these sites ofer stock price and volume changes on daily basis (OHLC).</t>
-  </si>
-  <si>
     <t>Downloaded stock data sample (whole year 2012 - subject to a change) for: Microsoft, Google, Cisco, Citybank, Coca Cola, McDonald's, Walt Disney co.</t>
   </si>
   <si>
-    <t>Started with a basic line chart as a template for my assignment and embeded it into my solution</t>
-  </si>
-  <si>
-    <t>Cerated a function 'private void ReadStockData(String sFileName)' to read a data source file and to set that data as a basis for the chart</t>
-  </si>
-  <si>
     <t>Referenced SciChart library within the project</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
   </si>
   <si>
     <t>Introduced DateTime type data as the X axis base - for a single stock, with no possibility to choose</t>
-  </si>
-  <si>
-    <t>Canceled the idea to introduce the scaling of the chart in order to corespond to data values - it is performed automatically</t>
   </si>
   <si>
     <t>The step of showing several prices at the same time (open, high, low and close price) is skipped - performed automatically by the SciChart</t>
@@ -201,6 +189,42 @@
   </si>
   <si>
     <t>Changed ReadStockData - much more elegant code...now it splits file into an array of string rows and each of them into arrays of string elements</t>
+  </si>
+  <si>
+    <t>DAY 4</t>
+  </si>
+  <si>
+    <t>Rearranged the project in terms of correct GitHub usage</t>
+  </si>
+  <si>
+    <t>Created a new branch VolumeTask</t>
+  </si>
+  <si>
+    <t>Introduced Tuple as the data structure used to sort our source data</t>
+  </si>
+  <si>
+    <t>Imported System.Collections.Generic in order to use the list of tuples</t>
+  </si>
+  <si>
+    <t>Data source doesn't have to be presorted anymore!</t>
+  </si>
+  <si>
+    <t>Downloaded freely available data samples from different web sites. All of these sites offer stock price and volume changes on daily basis (OHLC).</t>
+  </si>
+  <si>
+    <t>Started with a basic line chart as a template for my assignment and embedded it into my solution</t>
+  </si>
+  <si>
+    <t>Created a function 'private void ReadStockData(String sFileName)' to read a data source file and to set that data as a basis for the chart</t>
+  </si>
+  <si>
+    <t>Canceled the idea to introduce the scaling of the chart in order to correspond to data values - it is performed automatically</t>
+  </si>
+  <si>
+    <t>Because of scaling issue introduced checkbox control to give the possibility to the user to choose the way of volume data presentation</t>
+  </si>
+  <si>
+    <t>Embedded the control of data file's structure</t>
   </si>
 </sst>
 </file>
@@ -808,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -910,6 +934,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -946,46 +1007,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1289,11 +1314,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="24" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <pane ySplit="24" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1389,17 +1414,17 @@
       <c r="I10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="61"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="52" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1411,17 +1436,17 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="53"/>
+      <c r="J11" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="66"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="57"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
@@ -1431,15 +1456,15 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="57"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -1449,15 +1474,15 @@
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="50"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="63"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="53" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
@@ -1469,17 +1494,17 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="47"/>
+      <c r="J14" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="57"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25" t="s">
         <v>13</v>
@@ -1489,15 +1514,15 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="63"/>
     </row>
     <row r="16" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="57"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="26"/>
       <c r="D16" s="20"/>
       <c r="E16" s="27" t="s">
@@ -1507,17 +1532,17 @@
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="47"/>
+      <c r="J16" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="60"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="22"/>
@@ -1529,15 +1554,15 @@
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="50"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="63"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="57"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="24"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1547,17 +1572,17 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="47"/>
+      <c r="J18" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
     </row>
     <row r="19" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="57"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="26"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1567,15 +1592,15 @@
         <v>13</v>
       </c>
       <c r="I19" s="21"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="50"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="63"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="53" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="31"/>
@@ -1587,15 +1612,15 @@
       <c r="I20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="69"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="57"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="34"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1605,15 +1630,15 @@
       <c r="I21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="69"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="57"/>
     </row>
     <row r="22" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="58"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="36"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -1623,12 +1648,12 @@
       <c r="I22" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="65"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="70"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="48"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C24" s="40" t="s">
@@ -1696,120 +1721,168 @@
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="41"/>
       <c r="C34" s="5" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="41"/>
       <c r="C35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="41"/>
       <c r="C36" s="42" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="41"/>
       <c r="C37" s="42" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="41"/>
       <c r="C38" s="42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="41"/>
       <c r="C41" s="42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="41"/>
       <c r="C42" s="42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="41"/>
       <c r="C43" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="41"/>
       <c r="C44" s="43" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="H44" s="44"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="41"/>
       <c r="C45" s="43" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="41"/>
       <c r="C46" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="39"/>
       <c r="C47" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B48" s="38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="41"/>
       <c r="C49" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="41"/>
       <c r="C50" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="39"/>
       <c r="C51" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="41"/>
+      <c r="C53" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="41"/>
+      <c r="C54" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="41"/>
+      <c r="C55" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="41"/>
+      <c r="C56" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57" s="41"/>
+      <c r="C57" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58" s="39"/>
+      <c r="C58" s="45" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="J10:O10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
@@ -1824,10 +1897,6 @@
     <mergeCell ref="J16:O17"/>
     <mergeCell ref="J11:O13"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Additional alterations of supporting files
</commit_message>
<xml_diff>
--- a/Trading visualization assignment - Work plan.xlsx
+++ b/Trading visualization assignment - Work plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Create additional control objects  for showing technical indicators</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Added overview element to the chart</t>
+  </si>
+  <si>
+    <t>DAY 6</t>
+  </si>
+  <si>
+    <t>Merged master with VolumeTask branch</t>
   </si>
 </sst>
 </file>
@@ -953,12 +959,21 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -974,9 +989,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1024,12 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="24" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pane ySplit="24" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1432,17 +1438,17 @@
       <c r="I10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="49" t="s">
+      <c r="J10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="55" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1454,17 +1460,17 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="68"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="53"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
@@ -1474,15 +1480,15 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="71"/>
     </row>
     <row r="13" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="53"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="19" t="s">
         <v>13</v>
       </c>
@@ -1492,15 +1498,15 @@
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="65"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="22"/>
@@ -1512,17 +1518,17 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="60"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="62"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="53"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25" t="s">
         <v>13</v>
@@ -1532,15 +1538,15 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="65"/>
     </row>
     <row r="16" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="53"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="26"/>
       <c r="D16" s="20"/>
       <c r="E16" s="27" t="s">
@@ -1550,17 +1556,17 @@
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="58" t="s">
+      <c r="J16" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="60"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="62"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="46" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="22"/>
@@ -1572,15 +1578,15 @@
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="65"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="53"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="24"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1590,17 +1596,17 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="58" t="s">
+      <c r="J18" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="60"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="62"/>
     </row>
     <row r="19" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="53"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="26"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1610,15 +1616,15 @@
         <v>13</v>
       </c>
       <c r="I19" s="21"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="65"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="46" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="31"/>
@@ -1630,15 +1636,15 @@
       <c r="I20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="59"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="53"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="34"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1648,15 +1654,15 @@
       <c r="I21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="57"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="59"/>
     </row>
     <row r="22" spans="2:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="70"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="36"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -1666,12 +1672,12 @@
       <c r="I22" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="71"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="51"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C24" s="40" t="s">
@@ -1927,8 +1933,18 @@
         <v>71</v>
       </c>
     </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B64" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J11:O13"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="L22:M22"/>
@@ -1945,8 +1961,6 @@
     <mergeCell ref="J18:O19"/>
     <mergeCell ref="J14:O15"/>
     <mergeCell ref="J16:O17"/>
-    <mergeCell ref="J11:O13"/>
-    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>